<commit_message>
Se modifica formulario para enviar contraseña antes de cifrado a correo
</commit_message>
<xml_diff>
--- a/QYMSAS/bin/Debug/temp/facopio.xlsx
+++ b/QYMSAS/bin/Debug/temp/facopio.xlsx
@@ -41,13 +41,13 @@
     <x:t>FECHA INICIAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>1/06/2021</x:t>
+    <x:t>1/01/2021</x:t>
   </x:si>
   <x:si>
     <x:t>FECHA FINAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>3/06/2021</x:t>
+    <x:t>4/06/2021</x:t>
   </x:si>
   <x:si>
     <x:t>ACOPIO LA QUICA</x:t>
@@ -1117,7 +1117,7 @@
       <x:c r="I14" s="17" t="s"/>
       <x:c r="J14" s="17" t="s"/>
       <x:c r="K14" s="18" t="n">
-        <x:v>0</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="L14" s="18" t="s"/>
       <x:c r="M14" s="19" t="s"/>
@@ -1136,7 +1136,7 @@
       <x:c r="I15" s="17" t="s"/>
       <x:c r="J15" s="17" t="s"/>
       <x:c r="K15" s="18" t="n">
-        <x:v>0</x:v>
+        <x:v>16000000</x:v>
       </x:c>
       <x:c r="L15" s="18" t="s"/>
       <x:c r="M15" s="19" t="s"/>
@@ -1163,7 +1163,7 @@
       <x:c r="I17" s="17" t="s"/>
       <x:c r="J17" s="17" t="s"/>
       <x:c r="K17" s="18" t="n">
-        <x:v>0</x:v>
+        <x:v>559300</x:v>
       </x:c>
       <x:c r="L17" s="18" t="s"/>
       <x:c r="M17" s="19" t="s"/>
@@ -1190,7 +1190,7 @@
       <x:c r="I19" s="17" t="s"/>
       <x:c r="J19" s="17" t="s"/>
       <x:c r="K19" s="18" t="n">
-        <x:v>0</x:v>
+        <x:v>9800000</x:v>
       </x:c>
       <x:c r="L19" s="18" t="s"/>
       <x:c r="M19" s="19" t="s"/>

</xml_diff>